<commit_message>
Updated the rubric, wrote new instructions for next year.
</commit_message>
<xml_diff>
--- a/Labs/Lab3/Assignment3Rubric.xlsx
+++ b/Labs/Lab3/Assignment3Rubric.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Repos\CS246-CourseMaterials\Labs\Lab3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS246-CourseMaterials/Labs/Lab3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C059EE-E74D-41F1-A3BB-04BBA7084655}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CA48DDF9-C0DB-684A-B75A-BEA8218AFEF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14760" yWindow="495" windowWidth="10620" windowHeight="14640" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
+    <workbookView xWindow="9660" yWindow="500" windowWidth="13500" windowHeight="14640" activeTab="1" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
     <sheet name="Grade" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>Requirements</t>
   </si>
@@ -40,44 +40,35 @@
     <t>Total</t>
   </si>
   <si>
-    <t>CS246 Assignment 5 Rubric</t>
-  </si>
-  <si>
-    <t>Software Proposal for a Real Client</t>
-  </si>
-  <si>
-    <t>5A Proposal</t>
-  </si>
-  <si>
-    <t>5B Contract</t>
-  </si>
-  <si>
-    <t>Cover letter</t>
-  </si>
-  <si>
-    <t>Subtotal</t>
-  </si>
-  <si>
-    <t>Project overview</t>
-  </si>
-  <si>
-    <t>Estimate</t>
-  </si>
-  <si>
-    <t>Deployment &amp; Documentation</t>
-  </si>
-  <si>
-    <t>Cost and terms</t>
-  </si>
-  <si>
-    <t>Timeframe &amp; workflow</t>
+    <t>CS246 Assignment 3 Rubric</t>
+  </si>
+  <si>
+    <t>UX Design and Testing</t>
+  </si>
+  <si>
+    <t>UX Wireframes (1 per member)</t>
+  </si>
+  <si>
+    <t>Testing report</t>
+  </si>
+  <si>
+    <t>Test method description</t>
+  </si>
+  <si>
+    <t>Results of testing</t>
+  </si>
+  <si>
+    <t>Assessment of results quality</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -125,6 +116,20 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -155,6 +160,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,35 +479,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCD13E5-EC24-C14D-9BEE-EA2BBE4DEF6B}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B20"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="23.625" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,108 +515,80 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="B5" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="5" customFormat="1">
+      <c r="A6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="B7" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="4" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B10" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2">
-        <f>SUM(B6:B11)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <f>SUM(B5:B9)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="4"/>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="4"/>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="4"/>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="2">
-        <f>SUM(B15:B17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="2">
-        <f>SUM(B6:B17)</f>
-        <v>100</v>
-      </c>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -616,66 +598,75 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8EF6DB9-5046-F545-B378-AB8AF91CAAF1}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B20"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" customWidth="1"/>
+    <col min="4" max="4" width="1.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="E4" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="B5" s="2">
+        <v>50</v>
+      </c>
+      <c r="C5" s="2">
+        <v>50</v>
+      </c>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" s="2">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="B7" s="2">
         <v>10</v>
@@ -683,116 +674,96 @@
       <c r="C7" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="4" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B11" s="2">
-        <v>5</v>
+        <f>SUM(B5:B9)</f>
+        <v>100</v>
       </c>
       <c r="C11" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2">
-        <f>SUM(B6:B11)</f>
-        <v>50</v>
-      </c>
-      <c r="C12" s="2">
-        <f>SUM(C6:C11)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <f>SUM(C5:C9)</f>
+        <v>100</v>
+      </c>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" s="5" customFormat="1">
       <c r="A13" s="4"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
+      <c r="A14" s="4"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="4"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="4"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="2">
-        <f>SUM(B15:B17)</f>
-        <v>0</v>
-      </c>
-      <c r="C18" s="2">
-        <f>SUM(C15:C17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="2">
-        <f>SUM(B6:B17)</f>
-        <v>100</v>
-      </c>
-      <c r="C20" s="2">
-        <f>SUM(C6:C17)</f>
-        <v>100</v>
-      </c>
+    <row r="18" spans="1:3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revisions for next year
</commit_message>
<xml_diff>
--- a/Labs/Lab3/Assignment3Rubric.xlsx
+++ b/Labs/Lab3/Assignment3Rubric.xlsx
@@ -1,32 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS246-CourseMaterials/Labs/Lab3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS246-CourseMaterials\Labs\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CA48DDF9-C0DB-684A-B75A-BEA8218AFEF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1683CFA8-B281-4326-9F09-7455D6F38222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9660" yWindow="500" windowWidth="13500" windowHeight="14640" activeTab="1" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
+    <workbookView xWindow="-16212" yWindow="5676" windowWidth="15468" windowHeight="10992" activeTab="1" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
     <sheet name="Grade" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>Requirements</t>
   </si>
@@ -62,13 +73,16 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>UX diagrams (min 2 per member)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -183,9 +197,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -223,7 +237,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -329,7 +343,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -471,7 +485,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -485,29 +499,29 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -523,13 +537,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="5" customFormat="1">
+    <row r="6" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -537,7 +551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -545,7 +559,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -553,7 +567,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
@@ -562,31 +576,31 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="2"/>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
     </row>
@@ -601,36 +615,36 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" customWidth="1"/>
-    <col min="4" max="4" width="1.1640625" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.296875" customWidth="1"/>
+    <col min="2" max="2" width="9.296875" customWidth="1"/>
+    <col min="3" max="3" width="6.796875" customWidth="1"/>
+    <col min="4" max="4" width="1.19921875" customWidth="1"/>
+    <col min="5" max="5" width="18.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
@@ -644,9 +658,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2">
         <v>50</v>
@@ -656,7 +670,7 @@
       </c>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
@@ -664,7 +678,7 @@
       <c r="C6" s="2"/>
       <c r="E6" s="9"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -676,7 +690,7 @@
       </c>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -688,7 +702,7 @@
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -700,13 +714,13 @@
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
@@ -720,47 +734,47 @@
       </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:5" s="5" customFormat="1">
+    <row r="13" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>

</xml_diff>

<commit_message>
Updated intsructions and rubric
</commit_message>
<xml_diff>
--- a/Labs/Lab3/Assignment3Rubric.xlsx
+++ b/Labs/Lab3/Assignment3Rubric.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS246-CourseMaterials\Labs\Lab3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS246-CourseMaterials/Labs/Lab3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1683CFA8-B281-4326-9F09-7455D6F38222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C873B974-9D13-7545-82DB-376891B00ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16212" yWindow="5676" windowWidth="15468" windowHeight="10992" activeTab="1" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
+    <workbookView xWindow="-21280" yWindow="1980" windowWidth="16480" windowHeight="13400" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>UX Design and Testing</t>
   </si>
   <si>
-    <t>UX Wireframes (1 per member)</t>
-  </si>
-  <si>
     <t>Testing report</t>
   </si>
   <si>
@@ -75,14 +72,17 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>UX diagrams (min 2 per member)</t>
+    <t>UX diagrams</t>
+  </si>
+  <si>
+    <t>UX Wireframes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -495,33 +495,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCD13E5-EC24-C14D-9BEE-EA2BBE4DEF6B}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="23.69921875" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -529,45 +529,45 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" s="5" customFormat="1">
       <c r="A6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
@@ -576,31 +576,31 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" s="4"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" s="4"/>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" s="4"/>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" s="4"/>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" s="4"/>
       <c r="B16" s="2"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
     </row>
@@ -614,37 +614,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8EF6DB9-5046-F545-B378-AB8AF91CAAF1}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="28.296875" customWidth="1"/>
-    <col min="2" max="2" width="9.296875" customWidth="1"/>
-    <col min="3" max="3" width="6.796875" customWidth="1"/>
-    <col min="4" max="4" width="1.19921875" customWidth="1"/>
-    <col min="5" max="5" width="18.296875" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" customWidth="1"/>
+    <col min="4" max="4" width="1.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
@@ -655,12 +655,12 @@
         <v>2</v>
       </c>
       <c r="E4" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="B5" s="2">
         <v>50</v>
@@ -670,17 +670,17 @@
       </c>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="E6" s="9"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2">
         <v>10</v>
@@ -690,9 +690,9 @@
       </c>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
         <v>30</v>
@@ -702,9 +702,9 @@
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2">
         <v>10</v>
@@ -714,13 +714,13 @@
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" s="4"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
@@ -734,47 +734,47 @@
       </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" s="4"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" s="5" customFormat="1">
       <c r="A13" s="4"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="A14" s="4"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" s="4"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17" s="4"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18" s="4"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19" s="4"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>

</xml_diff>